<commit_message>
modify pinsport api function
</commit_message>
<xml_diff>
--- a/match_helper/match_helper/data/sql/create table/Table.xlsx
+++ b/match_helper/match_helper/data/sql/create table/Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="7" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,17 @@
     <sheet name="future_match" sheetId="13" r:id="rId12"/>
     <sheet name="teams_log" sheetId="14" r:id="rId13"/>
     <sheet name="names" sheetId="15" r:id="rId14"/>
-    <sheet name="mix_log" sheetId="16" r:id="rId15"/>
+    <sheet name="pin_sports" sheetId="16" r:id="rId15"/>
+    <sheet name="pin_leagues" sheetId="17" r:id="rId16"/>
+    <sheet name="pin_events" sheetId="18" r:id="rId17"/>
+    <sheet name="Sheet3" sheetId="19" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="167">
   <si>
     <t>timespan</t>
   </si>
@@ -513,6 +516,27 @@
   </si>
   <si>
     <t>eng_name</t>
+  </si>
+  <si>
+    <t>sport_id</t>
+  </si>
+  <si>
+    <t>sport_name</t>
+  </si>
+  <si>
+    <t>league_name</t>
+  </si>
+  <si>
+    <t>league_id</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>away</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1379,15 +1403,16 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1398,9 +1423,163 @@
         <v>129</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add new frm and table
</commit_message>
<xml_diff>
--- a/match_helper/match_helper/data/sql/create table/Table.xlsx
+++ b/match_helper/match_helper/data/sql/create table/Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="8" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,15 @@
     <sheet name="pin_sports" sheetId="16" r:id="rId15"/>
     <sheet name="pin_leagues" sheetId="17" r:id="rId16"/>
     <sheet name="pin_events" sheetId="18" r:id="rId17"/>
-    <sheet name="Sheet3" sheetId="19" r:id="rId18"/>
+    <sheet name="mbook_event" sheetId="20" r:id="rId18"/>
+    <sheet name="mbook_market" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="125725" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="177">
   <si>
     <t>timespan</t>
   </si>
@@ -537,6 +538,36 @@
   </si>
   <si>
     <t>away</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
+  <si>
+    <t>market_name</t>
+  </si>
+  <si>
+    <t>runner_name</t>
+  </si>
+  <si>
+    <t>mbook_market</t>
+  </si>
+  <si>
+    <t>depth_no</t>
+  </si>
+  <si>
+    <t>mbook_events</t>
+  </si>
+  <si>
+    <t>odd</t>
+  </si>
+  <si>
+    <t>amount</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1573,12 +1604,184 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add marathonbet table and single frm
</commit_message>
<xml_diff>
--- a/match_helper/match_helper/data/sql/create table/Table.xlsx
+++ b/match_helper/match_helper/data/sql/create table/Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="8" activeTab="18"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="12" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,17 @@
     <sheet name="pin_events" sheetId="18" r:id="rId17"/>
     <sheet name="mbook_event" sheetId="20" r:id="rId18"/>
     <sheet name="mbook_market" sheetId="19" r:id="rId19"/>
+    <sheet name="mb_events" sheetId="21" r:id="rId20"/>
+    <sheet name="mb_odds" sheetId="22" r:id="rId21"/>
+    <sheet name="temp_odds" sheetId="23" r:id="rId22"/>
+    <sheet name="Sheet4" sheetId="24" r:id="rId23"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="192">
   <si>
     <t>timespan</t>
   </si>
@@ -568,6 +572,51 @@
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>league</t>
+  </si>
+  <si>
+    <t>period_type</t>
+  </si>
+  <si>
+    <t>bet_type</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>o1</t>
+  </si>
+  <si>
+    <t>o2</t>
+  </si>
+  <si>
+    <t>o3</t>
+  </si>
+  <si>
+    <t>o4</t>
+  </si>
+  <si>
+    <t>o5</t>
+  </si>
+  <si>
+    <t>o6</t>
   </si>
 </sst>
 </file>
@@ -1694,7 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -2273,6 +2322,366 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>